<commit_message>
940408: configurator: update XL db (source: feurst_db_corr04042022-ob.xlsx OB 04/04/22)
</commit_message>
<xml_diff>
--- a/web/static/assets/data/feurst_db.xlsx
+++ b/web/static/assets/data/feurst_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\AA_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A790F396-8DAC-4325-8051-36AC8808E543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E995F43-29A3-44B3-99CD-664CF9ABF2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Machines" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10713" uniqueCount="1367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10733" uniqueCount="1367">
   <si>
     <t>TYPE DE MACHINE</t>
   </si>
@@ -51161,7 +51161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A15" sqref="A15:XFD16"/>
     </sheetView>
@@ -61097,9 +61097,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:X91"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U83" sqref="U83:X83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62945,7 +62945,18 @@
       <c r="T52" t="s">
         <v>1322</v>
       </c>
-      <c r="U52" s="57"/>
+      <c r="U52" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="V52" t="s">
+        <v>1322</v>
+      </c>
+      <c r="W52" t="s">
+        <v>1322</v>
+      </c>
+      <c r="X52" t="s">
+        <v>1322</v>
+      </c>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -63194,7 +63205,18 @@
       <c r="T59" t="s">
         <v>1329</v>
       </c>
-      <c r="U59" s="57"/>
+      <c r="U59" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="V59" t="s">
+        <v>1329</v>
+      </c>
+      <c r="W59" t="s">
+        <v>1329</v>
+      </c>
+      <c r="X59" t="s">
+        <v>1329</v>
+      </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -63443,7 +63465,18 @@
       <c r="T66" t="s">
         <v>1336</v>
       </c>
-      <c r="U66" s="57"/>
+      <c r="U66" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="V66" t="s">
+        <v>1336</v>
+      </c>
+      <c r="W66" t="s">
+        <v>1336</v>
+      </c>
+      <c r="X66" t="s">
+        <v>1336</v>
+      </c>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
@@ -63713,7 +63746,18 @@
       <c r="T74" t="s">
         <v>1344</v>
       </c>
-      <c r="U74" s="57"/>
+      <c r="U74" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="V74" t="s">
+        <v>1344</v>
+      </c>
+      <c r="W74" t="s">
+        <v>1344</v>
+      </c>
+      <c r="X74" t="s">
+        <v>1344</v>
+      </c>
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
@@ -64009,7 +64053,18 @@
       <c r="T83" t="s">
         <v>1353</v>
       </c>
-      <c r="U83" s="57"/>
+      <c r="U83" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="V83" t="s">
+        <v>1353</v>
+      </c>
+      <c r="W83" t="s">
+        <v>1353</v>
+      </c>
+      <c r="X83" t="s">
+        <v>1353</v>
+      </c>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84" t="s">

</xml_diff>